<commit_message>
fix menu and language
</commit_message>
<xml_diff>
--- a/public/templates/import_asset_template.xlsx
+++ b/public/templates/import_asset_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TokyoTechLab\ttlab-tims-web-app\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TokyoTechLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE198A4-7302-4AE3-A69E-3C7C29DD37CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF07A2D-91CB-456A-9B29-4AA45E9413D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{08182962-B681-49A5-8688-069F0687DFF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>15/03/2022</t>
   </si>
@@ -145,18 +145,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -474,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69AA391-BB82-46FA-A15C-DEF6E168215A}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +546,7 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="2">
@@ -558,7 +555,7 @@
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -584,7 +581,7 @@
       <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -607,59 +604,14 @@
       <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2">
-        <v>100000</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2">
-        <v>100000</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{92E64CBC-9F44-401C-8366-D40046EA158D}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{F4E905AF-D9E3-458A-8D9C-5DC89FB6AC62}">
       <formula1>"hardware, software"</formula1>
     </dataValidation>
@@ -669,7 +621,6 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{F4B18813-C9A0-49FE-B928-263CE18287FD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{92E64CBC-9F44-401C-8366-D40046EA158D}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{2E996F6D-5644-4020-8B21-6F613CFBA203}"/>

</xml_diff>